<commit_message>
middleware teacher & add createdBy attribute
</commit_message>
<xml_diff>
--- a/backend/excels/Cụm-trường-phía-Nam-Hưng-Yên---Đề-thi-thử-tốt-nghiệp-THPT-môn-Tiếng-Anh-năm-2022-2023.xlsx
+++ b/backend/excels/Cụm-trường-phía-Nam-Hưng-Yên---Đề-thi-thử-tốt-nghiệp-THPT-môn-Tiếng-Anh-năm-2022-2023.xlsx
@@ -2781,7 +2781,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="70.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="72">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="70.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="72">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="70.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="72">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
import excel câu hỏi
</commit_message>
<xml_diff>
--- a/backend/excels/Cụm-trường-phía-Nam-Hưng-Yên---Đề-thi-thử-tốt-nghiệp-THPT-môn-Tiếng-Anh-năm-2022-2023.xlsx
+++ b/backend/excels/Cụm-trường-phía-Nam-Hưng-Yên---Đề-thi-thử-tốt-nghiệp-THPT-môn-Tiếng-Anh-năm-2022-2023.xlsx
@@ -3767,7 +3767,7 @@
         <v>305</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="111.75">
       <c r="A36" s="1" t="s">
         <v>306</v>
       </c>
@@ -3796,7 +3796,7 @@
         <v>313</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="111.75">
       <c r="A37" s="1" t="s">
         <v>314</v>
       </c>
@@ -3825,7 +3825,7 @@
         <v>321</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="150.75">
       <c r="A38" s="1" t="s">
         <v>322</v>
       </c>
@@ -3852,7 +3852,7 @@
         <v>329</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="84.75">
       <c r="A39" s="1" t="s">
         <v>330</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>336</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="362.25">
       <c r="A40" s="1" t="s">
         <v>337</v>
       </c>
@@ -3908,7 +3908,7 @@
         <v>344</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="362.25">
       <c r="A41" s="1" t="s">
         <v>345</v>
       </c>
@@ -3937,7 +3937,7 @@
         <v>353</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="362.25">
       <c r="A42" s="1" t="s">
         <v>354</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>362</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="362.25">
       <c r="A43" s="1" t="s">
         <v>363</v>
       </c>
@@ -3995,7 +3995,7 @@
         <v>62</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="362.25">
       <c r="A44" s="1" t="s">
         <v>370</v>
       </c>
@@ -4024,7 +4024,7 @@
         <v>377</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="362.25">
       <c r="A45" s="1" t="s">
         <v>378</v>
       </c>
@@ -4053,7 +4053,7 @@
         <v>385</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="362.25">
       <c r="A46" s="1" t="s">
         <v>386</v>
       </c>
@@ -4082,7 +4082,7 @@
         <v>393</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="375.75">
       <c r="A47" s="1" t="s">
         <v>394</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>401</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="362.25">
       <c r="A48" s="1" t="s">
         <v>402</v>
       </c>
@@ -4140,7 +4140,7 @@
         <v>409</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="375.75">
       <c r="A49" s="1" t="s">
         <v>410</v>
       </c>
@@ -4169,7 +4169,7 @@
         <v>417</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="98.25">
       <c r="A50" s="1" t="s">
         <v>418</v>
       </c>
@@ -4196,7 +4196,7 @@
         <v>425</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="84.75">
       <c r="A51" s="1" t="s">
         <v>426</v>
       </c>

</xml_diff>